<commit_message>
Add live MF NAV fetching, reorder columns, and add annualized returns
- Fetch live NAV from Google Finance for all mutual funds
- Reorder main table: Units, Avg NAV, Current NAV, Current Value, Invested, P&L
- Reorder held lots: Buy Date, Units, Buy NAV, Current NAV, Cost, Current Value, P&L
- Add Cost and Sale Value columns to redemptions table
- Add duration and % p.a. to unrealized P&L in main table
- Fix step validation on AddMFModal inputs

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Mutual Funds/SBI Small Cap Fund - Direct Growth.xlsx
+++ b/dumps/Mutual Funds/SBI Small Cap Fund - Direct Growth.xlsx
@@ -878,7 +878,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN835"/>
+  <dimension ref="A1:AN837"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
@@ -1217,193 +1217,66 @@
       <c r="AN4" s="73" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="49" t="n">
-        <v>45565</v>
-      </c>
-      <c r="B5" s="50" t="inlineStr">
+      <c r="A5" s="120" t="n">
+        <v>46063</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>NSE</t>
         </is>
       </c>
-      <c r="C5" s="51" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Buy</t>
         </is>
       </c>
-      <c r="D5" s="52">
-        <f>F5/E5</f>
-        <v/>
-      </c>
-      <c r="E5" s="53" t="n">
-        <v>211.7156</v>
-      </c>
-      <c r="F5" s="54" t="n">
-        <v>25000</v>
-      </c>
-      <c r="G5" s="50" t="inlineStr">
+      <c r="D5" t="n">
+        <v>26.451</v>
+      </c>
+      <c r="E5" t="n">
+        <v>189.019</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4999.74</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
-          <t>SIP Purchase</t>
+          <t>~</t>
         </is>
       </c>
-      <c r="H5" s="55" t="n"/>
-      <c r="I5" s="55" t="n"/>
-      <c r="J5" s="56">
-        <f>Index!$C$2</f>
-        <v/>
-      </c>
-      <c r="K5" s="57">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), L5/sum(F5:I5), "")</f>
-        <v/>
-      </c>
-      <c r="L5" s="58">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
-        <v/>
-      </c>
-      <c r="M5" s="58">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), ((E5*D5)+L5), "")</f>
-        <v/>
-      </c>
-      <c r="N5" s="59">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), D5, "")</f>
-        <v/>
-      </c>
-      <c r="O5" s="57">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365, A5&lt;TODAY()-365*Index!$J$1), P5/sum(F5:I5), "")</f>
-        <v/>
-      </c>
-      <c r="P5" s="58">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365, A5&lt;TODAY()-365*Index!$J$1), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
-        <v/>
-      </c>
-      <c r="Q5" s="58">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365, A5&lt;TODAY()-365*Index!$J$1), ((E5*D5)+P5), "")</f>
-        <v/>
-      </c>
-      <c r="R5" s="58">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365, A5&lt;TODAY()-365*Index!$J$1), D5, "")</f>
-        <v/>
-      </c>
-      <c r="S5" s="57">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365, A5&lt;TODAY()-365*Index!$J$1), T5/sum(F5:I5), "")</f>
-        <v/>
-      </c>
-      <c r="T5" s="58">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365, A5&lt;TODAY()-365*Index!$J$1), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
-        <v/>
-      </c>
-      <c r="U5" s="58">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365, A5&lt;TODAY()-365*Index!$J$1), ((E5*D5)+T5), "")</f>
-        <v/>
-      </c>
-      <c r="V5" s="58">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365, A5&lt;TODAY()-365*Index!$J$1), D5, "")</f>
-        <v/>
-      </c>
-      <c r="W5" s="16" t="n"/>
-      <c r="X5" s="16" t="n"/>
-      <c r="Y5" s="60">
-        <f>IF(AND( C5="Buy", W5&lt;&gt;"", AA5&lt;&gt;"", B5&lt;&gt;"DIV"), Z5/sum(F5:I5), "")</f>
-        <v/>
-      </c>
-      <c r="Z5" s="16" t="n"/>
-      <c r="AA5" s="16" t="n"/>
-      <c r="AB5" s="61" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="49" t="n">
-        <v>45421</v>
-      </c>
-      <c r="B6" s="50" t="inlineStr">
+      <c r="A6" s="120" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>NSE</t>
         </is>
       </c>
-      <c r="C6" s="51" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
       </c>
-      <c r="D6" s="52" t="n">
-        <v>28.574</v>
-      </c>
-      <c r="E6" s="53" t="n">
-        <v>174.98</v>
-      </c>
-      <c r="F6" s="54" t="n">
-        <v>4999.75</v>
-      </c>
-      <c r="G6" s="50" t="inlineStr">
+      <c r="D6" s="0" t="n">
+        <v>26.854</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>186.1837</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>4999.78</v>
+      </c>
+      <c r="G6" s="0" t="inlineStr">
         <is>
-          <t>SIP Purchase</t>
+          <t>~</t>
         </is>
       </c>
-      <c r="H6" s="55" t="n"/>
-      <c r="I6" s="55" t="n"/>
-      <c r="J6" s="56">
-        <f>Index!$C$2</f>
-        <v/>
-      </c>
-      <c r="K6" s="57">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), L6/sum(F6:I6), "")</f>
-        <v/>
-      </c>
-      <c r="L6" s="58">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
-        <v/>
-      </c>
-      <c r="M6" s="58">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), ((E6*D6)+L6), "")</f>
-        <v/>
-      </c>
-      <c r="N6" s="59">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), D6, "")</f>
-        <v/>
-      </c>
-      <c r="O6" s="57">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365, A6&lt;TODAY()-365*Index!$J$1), P6/sum(F6:I6), "")</f>
-        <v/>
-      </c>
-      <c r="P6" s="58">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365, A6&lt;TODAY()-365*Index!$J$1), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
-        <v/>
-      </c>
-      <c r="Q6" s="58">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365, A6&lt;TODAY()-365*Index!$J$1), ((E6*D6)+P6), "")</f>
-        <v/>
-      </c>
-      <c r="R6" s="58">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365, A6&lt;TODAY()-365*Index!$J$1), D6, "")</f>
-        <v/>
-      </c>
-      <c r="S6" s="57">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365, A6&lt;TODAY()-365*Index!$J$1), T6/sum(F6:I6), "")</f>
-        <v/>
-      </c>
-      <c r="T6" s="58">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365, A6&lt;TODAY()-365*Index!$J$1), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
-        <v/>
-      </c>
-      <c r="U6" s="58">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365, A6&lt;TODAY()-365*Index!$J$1), ((E6*D6)+T6), "")</f>
-        <v/>
-      </c>
-      <c r="V6" s="58">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365, A6&lt;TODAY()-365*Index!$J$1), D6, "")</f>
-        <v/>
-      </c>
-      <c r="W6" s="16" t="n"/>
-      <c r="X6" s="16" t="n"/>
-      <c r="Y6" s="60">
-        <f>IF(AND( C6="Buy", W6&lt;&gt;"", AA6&lt;&gt;"", B6&lt;&gt;"DIV"), Z6/sum(F6:I6), "")</f>
-        <v/>
-      </c>
-      <c r="Z6" s="16" t="n"/>
-      <c r="AA6" s="16" t="n"/>
-      <c r="AB6" s="61" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="49" t="n">
-        <v>45392</v>
+        <v>45565</v>
       </c>
       <c r="B7" s="50" t="inlineStr">
         <is>
@@ -1412,103 +1285,91 @@
       </c>
       <c r="C7" s="51" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
-      <c r="D7" s="52" t="n">
-        <v>28.26</v>
+      <c r="D7" s="52">
+        <f>F5/E5</f>
+        <v/>
       </c>
       <c r="E7" s="53" t="n">
-        <v>176.92</v>
+        <v>211.7156</v>
       </c>
       <c r="F7" s="54" t="n">
-        <v>4999.75</v>
+        <v>25000</v>
       </c>
       <c r="G7" s="50" t="inlineStr">
         <is>
           <t>SIP Purchase</t>
         </is>
       </c>
-      <c r="H7" s="62" t="n"/>
-      <c r="I7" s="62" t="n"/>
+      <c r="H7" s="55" t="n"/>
+      <c r="I7" s="55" t="n"/>
       <c r="J7" s="56">
         <f>Index!$C$2</f>
         <v/>
       </c>
-      <c r="K7" s="63">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), L7/sum(F7:I7), "")</f>
+      <c r="K7" s="57">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), L5/sum(F5:I5), "")</f>
         <v/>
       </c>
-      <c r="L7" s="16">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
+      <c r="L7" s="58">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
         <v/>
       </c>
-      <c r="M7" s="16">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), ((E7*D7)+L7), "")</f>
+      <c r="M7" s="58">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), ((E5*D5)+L5), "")</f>
         <v/>
       </c>
-      <c r="N7" s="61">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), D7, "")</f>
+      <c r="N7" s="59">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), D5, "")</f>
         <v/>
       </c>
-      <c r="O7" s="63">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), P7/sum(F7:I7), "")</f>
+      <c r="O7" s="57">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365, A5&lt;TODAY()-365*Index!$J$1), P5/sum(F5:I5), "")</f>
         <v/>
       </c>
-      <c r="P7" s="16">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
+      <c r="P7" s="58">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365, A5&lt;TODAY()-365*Index!$J$1), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
         <v/>
       </c>
-      <c r="Q7" s="16">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), ((E7*D7)+P7), "")</f>
+      <c r="Q7" s="58">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365, A5&lt;TODAY()-365*Index!$J$1), ((E5*D5)+P5), "")</f>
         <v/>
       </c>
-      <c r="R7" s="16">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), D7, "")</f>
+      <c r="R7" s="58">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365, A5&lt;TODAY()-365*Index!$J$1), D5, "")</f>
         <v/>
       </c>
-      <c r="S7" s="63">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), T7/sum(F7:I7), "")</f>
+      <c r="S7" s="57">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365, A5&lt;TODAY()-365*Index!$J$1), T5/sum(F5:I5), "")</f>
         <v/>
       </c>
-      <c r="T7" s="16">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
+      <c r="T7" s="58">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365, A5&lt;TODAY()-365*Index!$J$1), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
         <v/>
       </c>
-      <c r="U7" s="16">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), ((E7*D7)+T7), "")</f>
+      <c r="U7" s="58">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365, A5&lt;TODAY()-365*Index!$J$1), ((E5*D5)+T5), "")</f>
         <v/>
       </c>
-      <c r="V7" s="16">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), D7, "")</f>
+      <c r="V7" s="58">
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365, A5&lt;TODAY()-365*Index!$J$1), D5, "")</f>
         <v/>
       </c>
-      <c r="W7" s="53" t="n">
-        <v>211.7156</v>
-      </c>
-      <c r="X7" s="49" t="n">
-        <v>45565</v>
-      </c>
-      <c r="Y7" s="64">
-        <f>IF(AND( C7="Buy", W7&lt;&gt;"", AA7&lt;&gt;"", B7&lt;&gt;"DIV"), Z7/sum(F7:I7), "")</f>
+      <c r="W7" s="16" t="n"/>
+      <c r="X7" s="16" t="n"/>
+      <c r="Y7" s="60">
+        <f>IF(AND( C5="Buy", W5&lt;&gt;"", AA5&lt;&gt;"", B5&lt;&gt;"DIV"), Z5/sum(F5:I5), "")</f>
         <v/>
       </c>
-      <c r="Z7" s="65">
-        <f>(1-Index!$F$2*2)*((W7*D7)-(E7*D7))</f>
-        <v/>
-      </c>
-      <c r="AA7" s="65">
-        <f>((E7*D7)+Z7)</f>
-        <v/>
-      </c>
-      <c r="AB7" s="66">
-        <f>D7</f>
-        <v/>
-      </c>
+      <c r="Z7" s="16" t="n"/>
+      <c r="AA7" s="16" t="n"/>
+      <c r="AB7" s="61" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="49" t="n">
-        <v>45362</v>
+        <v>45421</v>
       </c>
       <c r="B8" s="50" t="inlineStr">
         <is>
@@ -1521,10 +1382,10 @@
         </is>
       </c>
       <c r="D8" s="52" t="n">
-        <v>29.676</v>
+        <v>28.574</v>
       </c>
       <c r="E8" s="53" t="n">
-        <v>168.48</v>
+        <v>174.98</v>
       </c>
       <c r="F8" s="54" t="n">
         <v>4999.75</v>
@@ -1534,86 +1395,73 @@
           <t>SIP Purchase</t>
         </is>
       </c>
-      <c r="H8" s="62" t="n"/>
-      <c r="I8" s="62" t="n"/>
+      <c r="H8" s="55" t="n"/>
+      <c r="I8" s="55" t="n"/>
       <c r="J8" s="56">
         <f>Index!$C$2</f>
         <v/>
       </c>
-      <c r="K8" s="63">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), L8/sum(F8:I8), "")</f>
+      <c r="K8" s="57">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), L6/sum(F6:I6), "")</f>
         <v/>
       </c>
-      <c r="L8" s="16">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+      <c r="L8" s="58">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
         <v/>
       </c>
-      <c r="M8" s="16">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), ((E8*D8)+L8), "")</f>
+      <c r="M8" s="58">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), ((E6*D6)+L6), "")</f>
         <v/>
       </c>
-      <c r="N8" s="61">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), D8, "")</f>
+      <c r="N8" s="59">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), D6, "")</f>
         <v/>
       </c>
-      <c r="O8" s="63">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), P8/sum(F8:I8), "")</f>
+      <c r="O8" s="57">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365, A6&lt;TODAY()-365*Index!$J$1), P6/sum(F6:I6), "")</f>
         <v/>
       </c>
-      <c r="P8" s="16">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+      <c r="P8" s="58">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365, A6&lt;TODAY()-365*Index!$J$1), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
         <v/>
       </c>
-      <c r="Q8" s="16">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), ((E8*D8)+P8), "")</f>
+      <c r="Q8" s="58">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365, A6&lt;TODAY()-365*Index!$J$1), ((E6*D6)+P6), "")</f>
         <v/>
       </c>
-      <c r="R8" s="16">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), D8, "")</f>
+      <c r="R8" s="58">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365, A6&lt;TODAY()-365*Index!$J$1), D6, "")</f>
         <v/>
       </c>
-      <c r="S8" s="63">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), T8/sum(F8:I8), "")</f>
+      <c r="S8" s="57">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365, A6&lt;TODAY()-365*Index!$J$1), T6/sum(F6:I6), "")</f>
         <v/>
       </c>
-      <c r="T8" s="16">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+      <c r="T8" s="58">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365, A6&lt;TODAY()-365*Index!$J$1), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
         <v/>
       </c>
-      <c r="U8" s="16">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), ((E8*D8)+T8), "")</f>
+      <c r="U8" s="58">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365, A6&lt;TODAY()-365*Index!$J$1), ((E6*D6)+T6), "")</f>
         <v/>
       </c>
-      <c r="V8" s="16">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), D8, "")</f>
+      <c r="V8" s="58">
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365, A6&lt;TODAY()-365*Index!$J$1), D6, "")</f>
         <v/>
       </c>
-      <c r="W8" s="53" t="n">
-        <v>211.7156</v>
-      </c>
-      <c r="X8" s="49" t="n">
-        <v>45565</v>
-      </c>
-      <c r="Y8" s="64">
-        <f>IF(AND( C8="Buy", W8&lt;&gt;"", AA8&lt;&gt;"", B8&lt;&gt;"DIV"), Z8/sum(F8:I8), "")</f>
+      <c r="W8" s="16" t="n"/>
+      <c r="X8" s="16" t="n"/>
+      <c r="Y8" s="60">
+        <f>IF(AND( C6="Buy", W6&lt;&gt;"", AA6&lt;&gt;"", B6&lt;&gt;"DIV"), Z6/sum(F6:I6), "")</f>
         <v/>
       </c>
-      <c r="Z8" s="65">
-        <f>(1-Index!$F$2*2)*((W8*D8)-(E8*D8))</f>
-        <v/>
-      </c>
-      <c r="AA8" s="65">
-        <f>((E8*D8)+Z8)</f>
-        <v/>
-      </c>
-      <c r="AB8" s="66">
-        <f>D8</f>
-        <v/>
-      </c>
+      <c r="Z8" s="16" t="n"/>
+      <c r="AA8" s="16" t="n"/>
+      <c r="AB8" s="61" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="49" t="n">
-        <v>45327</v>
+        <v>45392</v>
       </c>
       <c r="B9" s="50" t="inlineStr">
         <is>
@@ -1626,10 +1474,10 @@
         </is>
       </c>
       <c r="D9" s="52" t="n">
-        <v>29.636</v>
+        <v>28.26</v>
       </c>
       <c r="E9" s="53" t="n">
-        <v>168.71</v>
+        <v>176.92</v>
       </c>
       <c r="F9" s="54" t="n">
         <v>4999.75</v>
@@ -1646,51 +1494,51 @@
         <v/>
       </c>
       <c r="K9" s="63">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), L9/sum(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), L7/sum(F7:I7), "")</f>
         <v/>
       </c>
       <c r="L9" s="16">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="M9" s="16">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), ((E9*D9)+L9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), ((E7*D7)+L7), "")</f>
         <v/>
       </c>
       <c r="N9" s="61">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), D7, "")</f>
         <v/>
       </c>
       <c r="O9" s="63">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), P9/sum(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), P7/sum(F7:I7), "")</f>
         <v/>
       </c>
       <c r="P9" s="16">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="Q9" s="16">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), ((E9*D9)+P9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), ((E7*D7)+P7), "")</f>
         <v/>
       </c>
       <c r="R9" s="16">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), D7, "")</f>
         <v/>
       </c>
       <c r="S9" s="63">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), T9/sum(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), T7/sum(F7:I7), "")</f>
         <v/>
       </c>
       <c r="T9" s="16">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="U9" s="16">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), ((E9*D9)+T9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), ((E7*D7)+T7), "")</f>
         <v/>
       </c>
       <c r="V9" s="16">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), D7, "")</f>
         <v/>
       </c>
       <c r="W9" s="53" t="n">
@@ -1700,25 +1548,25 @@
         <v>45565</v>
       </c>
       <c r="Y9" s="64">
-        <f>IF(AND( C9="Buy", W9&lt;&gt;"", AA9&lt;&gt;"", B9&lt;&gt;"DIV"), Z9/sum(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", W7&lt;&gt;"", AA7&lt;&gt;"", B7&lt;&gt;"DIV"), Z7/sum(F7:I7), "")</f>
         <v/>
       </c>
       <c r="Z9" s="65">
-        <f>(1-Index!$F$2*2)*((W9*D9)-(E9*D9))</f>
+        <f>(1-Index!$F$2*2)*((W7*D7)-(E7*D7))</f>
         <v/>
       </c>
       <c r="AA9" s="65">
-        <f>((E9*D9)+Z9)</f>
+        <f>((E7*D7)+Z7)</f>
         <v/>
       </c>
       <c r="AB9" s="66">
-        <f>D9</f>
+        <f>D7</f>
         <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="49" t="n">
-        <v>45296</v>
+        <v>45362</v>
       </c>
       <c r="B10" s="50" t="inlineStr">
         <is>
@@ -1731,10 +1579,10 @@
         </is>
       </c>
       <c r="D10" s="52" t="n">
-        <v>30.705</v>
+        <v>29.676</v>
       </c>
       <c r="E10" s="53" t="n">
-        <v>162.83</v>
+        <v>168.48</v>
       </c>
       <c r="F10" s="54" t="n">
         <v>4999.75</v>
@@ -1751,119 +1599,285 @@
         <v/>
       </c>
       <c r="K10" s="63">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), L8/sum(F8:I8), "")</f>
+        <v/>
+      </c>
+      <c r="L10" s="16">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+        <v/>
+      </c>
+      <c r="M10" s="16">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), ((E8*D8)+L8), "")</f>
+        <v/>
+      </c>
+      <c r="N10" s="61">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), D8, "")</f>
+        <v/>
+      </c>
+      <c r="O10" s="63">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), P8/sum(F8:I8), "")</f>
+        <v/>
+      </c>
+      <c r="P10" s="16">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+        <v/>
+      </c>
+      <c r="Q10" s="16">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), ((E8*D8)+P8), "")</f>
+        <v/>
+      </c>
+      <c r="R10" s="16">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), D8, "")</f>
+        <v/>
+      </c>
+      <c r="S10" s="63">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), T8/sum(F8:I8), "")</f>
+        <v/>
+      </c>
+      <c r="T10" s="16">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+        <v/>
+      </c>
+      <c r="U10" s="16">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), ((E8*D8)+T8), "")</f>
+        <v/>
+      </c>
+      <c r="V10" s="16">
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), D8, "")</f>
+        <v/>
+      </c>
+      <c r="W10" s="53" t="n">
+        <v>211.7156</v>
+      </c>
+      <c r="X10" s="49" t="n">
+        <v>45565</v>
+      </c>
+      <c r="Y10" s="64">
+        <f>IF(AND( C8="Buy", W8&lt;&gt;"", AA8&lt;&gt;"", B8&lt;&gt;"DIV"), Z8/sum(F8:I8), "")</f>
+        <v/>
+      </c>
+      <c r="Z10" s="65">
+        <f>(1-Index!$F$2*2)*((W8*D8)-(E8*D8))</f>
+        <v/>
+      </c>
+      <c r="AA10" s="65">
+        <f>((E8*D8)+Z8)</f>
+        <v/>
+      </c>
+      <c r="AB10" s="66">
+        <f>D8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="49" t="n">
+        <v>45327</v>
+      </c>
+      <c r="B11" s="50" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C11" s="51" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D11" s="52" t="n">
+        <v>29.636</v>
+      </c>
+      <c r="E11" s="53" t="n">
+        <v>168.71</v>
+      </c>
+      <c r="F11" s="54" t="n">
+        <v>4999.75</v>
+      </c>
+      <c r="G11" s="50" t="inlineStr">
+        <is>
+          <t>SIP Purchase</t>
+        </is>
+      </c>
+      <c r="H11" s="62" t="n"/>
+      <c r="I11" s="62" t="n"/>
+      <c r="J11" s="56">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+      <c r="K11" s="63">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), L9/sum(F9:I9), "")</f>
+        <v/>
+      </c>
+      <c r="L11" s="16">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <v/>
+      </c>
+      <c r="M11" s="16">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), ((E9*D9)+L9), "")</f>
+        <v/>
+      </c>
+      <c r="N11" s="61">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), D9, "")</f>
+        <v/>
+      </c>
+      <c r="O11" s="63">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), P9/sum(F9:I9), "")</f>
+        <v/>
+      </c>
+      <c r="P11" s="16">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <v/>
+      </c>
+      <c r="Q11" s="16">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), ((E9*D9)+P9), "")</f>
+        <v/>
+      </c>
+      <c r="R11" s="16">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), D9, "")</f>
+        <v/>
+      </c>
+      <c r="S11" s="63">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), T9/sum(F9:I9), "")</f>
+        <v/>
+      </c>
+      <c r="T11" s="16">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <v/>
+      </c>
+      <c r="U11" s="16">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), ((E9*D9)+T9), "")</f>
+        <v/>
+      </c>
+      <c r="V11" s="16">
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), D9, "")</f>
+        <v/>
+      </c>
+      <c r="W11" s="53" t="n">
+        <v>211.7156</v>
+      </c>
+      <c r="X11" s="49" t="n">
+        <v>45565</v>
+      </c>
+      <c r="Y11" s="64">
+        <f>IF(AND( C9="Buy", W9&lt;&gt;"", AA9&lt;&gt;"", B9&lt;&gt;"DIV"), Z9/sum(F9:I9), "")</f>
+        <v/>
+      </c>
+      <c r="Z11" s="65">
+        <f>(1-Index!$F$2*2)*((W9*D9)-(E9*D9))</f>
+        <v/>
+      </c>
+      <c r="AA11" s="65">
+        <f>((E9*D9)+Z9)</f>
+        <v/>
+      </c>
+      <c r="AB11" s="66">
+        <f>D9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="49" t="n">
+        <v>45296</v>
+      </c>
+      <c r="B12" s="50" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C12" s="51" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D12" s="52" t="n">
+        <v>30.705</v>
+      </c>
+      <c r="E12" s="53" t="n">
+        <v>162.83</v>
+      </c>
+      <c r="F12" s="54" t="n">
+        <v>4999.75</v>
+      </c>
+      <c r="G12" s="50" t="inlineStr">
+        <is>
+          <t>SIP Purchase</t>
+        </is>
+      </c>
+      <c r="H12" s="62" t="n"/>
+      <c r="I12" s="62" t="n"/>
+      <c r="J12" s="56">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+      <c r="K12" s="63">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), L10/sum(F10:I10), "")</f>
         <v/>
       </c>
-      <c r="L10" s="16">
+      <c r="L12" s="16">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
-      <c r="M10" s="16">
+      <c r="M12" s="16">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), ((E10*D10)+L10), "")</f>
         <v/>
       </c>
-      <c r="N10" s="61">
+      <c r="N12" s="61">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), D10, "")</f>
         <v/>
       </c>
-      <c r="O10" s="63">
+      <c r="O12" s="63">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), P10/sum(F10:I10), "")</f>
         <v/>
       </c>
-      <c r="P10" s="16">
+      <c r="P12" s="16">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
-      <c r="Q10" s="16">
+      <c r="Q12" s="16">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), ((E10*D10)+P10), "")</f>
         <v/>
       </c>
-      <c r="R10" s="16">
+      <c r="R12" s="16">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), D10, "")</f>
         <v/>
       </c>
-      <c r="S10" s="63">
+      <c r="S12" s="63">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), T10/sum(F10:I10), "")</f>
         <v/>
       </c>
-      <c r="T10" s="16">
+      <c r="T12" s="16">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
-      <c r="U10" s="16">
+      <c r="U12" s="16">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), ((E10*D10)+T10), "")</f>
         <v/>
       </c>
-      <c r="V10" s="16">
+      <c r="V12" s="16">
         <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), D10, "")</f>
         <v/>
       </c>
-      <c r="W10" s="53" t="n">
+      <c r="W12" s="53" t="n">
         <v>211.7156</v>
       </c>
-      <c r="X10" s="49" t="n">
+      <c r="X12" s="49" t="n">
         <v>45565</v>
       </c>
-      <c r="Y10" s="64">
+      <c r="Y12" s="64">
         <f>IF(AND( C10="Buy", W10&lt;&gt;"", AA10&lt;&gt;"", B10&lt;&gt;"DIV"), Z10/sum(F10:I10), "")</f>
         <v/>
       </c>
-      <c r="Z10" s="65">
+      <c r="Z12" s="65">
         <f>(1-Index!$F$2*2)*((W10*D10)-(E10*D10))</f>
         <v/>
       </c>
-      <c r="AA10" s="65">
+      <c r="AA12" s="65">
         <f>((E10*D10)+Z10)</f>
         <v/>
       </c>
-      <c r="AB10" s="66">
+      <c r="AB12" s="66">
         <f>D10</f>
         <v/>
       </c>
-    </row>
-    <row r="11">
-      <c r="D11" s="67" t="n"/>
-      <c r="E11" s="68" t="n"/>
-      <c r="F11" s="69" t="n"/>
-      <c r="G11" s="70" t="n"/>
-      <c r="J11" s="69" t="n"/>
-      <c r="K11" s="71" t="n"/>
-      <c r="L11" s="69" t="n"/>
-      <c r="O11" s="69" t="n"/>
-      <c r="P11" s="69" t="n"/>
-      <c r="Q11" s="69" t="n"/>
-      <c r="R11" s="69" t="n"/>
-      <c r="S11" s="69" t="n"/>
-      <c r="T11" s="69" t="n"/>
-      <c r="U11" s="69" t="n"/>
-      <c r="V11" s="69" t="n"/>
-      <c r="X11" s="69" t="n"/>
-      <c r="Y11" s="69" t="n"/>
-      <c r="Z11" s="69" t="n"/>
-      <c r="AA11" s="69" t="n"/>
-      <c r="AB11" s="68" t="n"/>
-    </row>
-    <row r="12">
-      <c r="D12" s="67" t="n"/>
-      <c r="E12" s="68" t="n"/>
-      <c r="F12" s="69" t="n"/>
-      <c r="G12" s="70" t="n"/>
-      <c r="J12" s="69" t="n"/>
-      <c r="K12" s="71" t="n"/>
-      <c r="L12" s="69" t="n"/>
-      <c r="O12" s="69" t="n"/>
-      <c r="P12" s="69" t="n"/>
-      <c r="Q12" s="69" t="n"/>
-      <c r="R12" s="69" t="n"/>
-      <c r="S12" s="69" t="n"/>
-      <c r="T12" s="69" t="n"/>
-      <c r="U12" s="69" t="n"/>
-      <c r="V12" s="69" t="n"/>
-      <c r="X12" s="69" t="n"/>
-      <c r="Y12" s="69" t="n"/>
-      <c r="Z12" s="69" t="n"/>
-      <c r="AA12" s="69" t="n"/>
-      <c r="AB12" s="68" t="n"/>
     </row>
     <row r="13">
       <c r="D13" s="67" t="n"/>
@@ -19970,6 +19984,50 @@
       <c r="Z835" s="69" t="n"/>
       <c r="AA835" s="69" t="n"/>
       <c r="AB835" s="68" t="n"/>
+    </row>
+    <row r="836">
+      <c r="D836" s="67" t="n"/>
+      <c r="E836" s="68" t="n"/>
+      <c r="F836" s="69" t="n"/>
+      <c r="G836" s="70" t="n"/>
+      <c r="J836" s="69" t="n"/>
+      <c r="K836" s="71" t="n"/>
+      <c r="L836" s="69" t="n"/>
+      <c r="O836" s="69" t="n"/>
+      <c r="P836" s="69" t="n"/>
+      <c r="Q836" s="69" t="n"/>
+      <c r="R836" s="69" t="n"/>
+      <c r="S836" s="69" t="n"/>
+      <c r="T836" s="69" t="n"/>
+      <c r="U836" s="69" t="n"/>
+      <c r="V836" s="69" t="n"/>
+      <c r="X836" s="69" t="n"/>
+      <c r="Y836" s="69" t="n"/>
+      <c r="Z836" s="69" t="n"/>
+      <c r="AA836" s="69" t="n"/>
+      <c r="AB836" s="68" t="n"/>
+    </row>
+    <row r="837">
+      <c r="D837" s="67" t="n"/>
+      <c r="E837" s="68" t="n"/>
+      <c r="F837" s="69" t="n"/>
+      <c r="G837" s="70" t="n"/>
+      <c r="J837" s="69" t="n"/>
+      <c r="K837" s="71" t="n"/>
+      <c r="L837" s="69" t="n"/>
+      <c r="O837" s="69" t="n"/>
+      <c r="P837" s="69" t="n"/>
+      <c r="Q837" s="69" t="n"/>
+      <c r="R837" s="69" t="n"/>
+      <c r="S837" s="69" t="n"/>
+      <c r="T837" s="69" t="n"/>
+      <c r="U837" s="69" t="n"/>
+      <c r="V837" s="69" t="n"/>
+      <c r="X837" s="69" t="n"/>
+      <c r="Y837" s="69" t="n"/>
+      <c r="Z837" s="69" t="n"/>
+      <c r="AA837" s="69" t="n"/>
+      <c r="AB837" s="68" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$4:$AL$10"/>

</xml_diff>